<commit_message>
FIX: support boolean value
</commit_message>
<xml_diff>
--- a/tests/UserCfgs.xlsx
+++ b/tests/UserCfgs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -44,6 +44,10 @@
   </si>
   <si>
     <t>zoro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>online</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -388,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -400,7 +404,7 @@
     <col min="5" max="5" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +420,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -432,6 +439,9 @@
       </c>
       <c r="E2" t="s">
         <v>6</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>